<commit_message>
Adicionando Banco de dados Cadastro usuario
</commit_message>
<xml_diff>
--- a/Streamlit_desafio_5/Modelo_Candidato_Simplificado.xlsx
+++ b/Streamlit_desafio_5/Modelo_Candidato_Simplificado.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\OneDrive\Documentos\GitHub\Fase-5-Challenge-Fiap\Streamlit_desafio_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{255763DA-954D-4F35-B241-2097C0EFBAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B492003-D5C3-4498-84C7-1AFA9E4FCD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
+    <t>Título da vaga desejada</t>
+  </si>
+  <si>
+    <t>Tipo da vaga desejada</t>
+  </si>
+  <si>
     <t>Área de interesse</t>
   </si>
   <si>
@@ -31,28 +37,22 @@
     <t>Nível de espanhol</t>
   </si>
   <si>
+    <t>Outros idiomas</t>
+  </si>
+  <si>
+    <t>Competências técnicas</t>
+  </si>
+  <si>
+    <t>Competências comportamentais</t>
+  </si>
+  <si>
+    <t>Disponível para viagens? (Sim/Não)</t>
+  </si>
+  <si>
+    <t>Possui equipamento próprio? (Sim/Não)</t>
+  </si>
+  <si>
     <t>Expectativa salarial</t>
-  </si>
-  <si>
-    <t>Skils técnicas</t>
-  </si>
-  <si>
-    <t>Competências a mais e certificacao</t>
-  </si>
-  <si>
-    <t>Nome completo</t>
-  </si>
-  <si>
-    <t>E-mail</t>
-  </si>
-  <si>
-    <t>Telefone</t>
-  </si>
-  <si>
-    <t>Formação acadêmica</t>
-  </si>
-  <si>
-    <t>Vaga de interesse</t>
   </si>
 </sst>
 </file>
@@ -423,55 +423,57 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>